<commit_message>
fix council display mode
</commit_message>
<xml_diff>
--- a/data/players_priorities.xlsx
+++ b/data/players_priorities.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scripts\Divide-BiS\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A068819-17A3-431A-97B1-90B52A500688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="119">
   <si>
     <t>player</t>
   </si>
@@ -37,33 +31,33 @@
     <t>received</t>
   </si>
   <si>
+    <t>Ninnah</t>
+  </si>
+  <si>
     <t>Queriss</t>
   </si>
   <si>
-    <t>Ninnah</t>
-  </si>
-  <si>
     <t>Aelvå</t>
   </si>
   <si>
+    <t>Ørly</t>
+  </si>
+  <si>
+    <t>Pamage</t>
+  </si>
+  <si>
+    <t>Pyrobifle</t>
+  </si>
+  <si>
     <t>Warloquë</t>
   </si>
   <si>
-    <t>Pamage</t>
-  </si>
-  <si>
-    <t>Ørly</t>
-  </si>
-  <si>
-    <t>Pyrobifle</t>
+    <t>Gosseyn</t>
   </si>
   <si>
     <t>Iryastra</t>
   </si>
   <si>
-    <t>Gosseyn</t>
-  </si>
-  <si>
     <t>Skotia</t>
   </si>
   <si>
@@ -376,14 +370,14 @@
     <t>Emblems of Conquest</t>
   </si>
   <si>
-    <t>x</t>
+    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -446,14 +440,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -500,7 +486,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -532,27 +518,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -584,24 +552,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -777,22 +727,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E187"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -809,7 +751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -822,11 +764,8 @@
       <c r="D2" t="s">
         <v>108</v>
       </c>
-      <c r="E2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -840,7 +779,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -854,7 +793,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -867,11 +806,8 @@
       <c r="D5" t="s">
         <v>108</v>
       </c>
-      <c r="E5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -885,7 +821,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -899,7 +835,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -913,7 +849,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -927,7 +863,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -941,9 +877,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>45135</v>
@@ -955,7 +891,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -969,9 +905,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B13">
         <v>45137</v>
@@ -983,9 +919,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B14">
         <v>45139</v>
@@ -997,9 +933,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15">
         <v>45145</v>
@@ -1011,7 +947,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1025,7 +961,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1039,9 +975,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B18">
         <v>45241</v>
@@ -1053,9 +989,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B19">
         <v>45241</v>
@@ -1067,9 +1003,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20">
         <v>45242</v>
@@ -1081,9 +1017,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21">
         <v>45242</v>
@@ -1095,9 +1031,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22">
         <v>45242</v>
@@ -1109,7 +1045,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -1123,7 +1059,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1137,9 +1073,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B25">
         <v>45247</v>
@@ -1151,9 +1087,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B26">
         <v>45250</v>
@@ -1165,9 +1101,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27">
         <v>45294</v>
@@ -1179,9 +1115,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B28">
         <v>45294</v>
@@ -1193,7 +1129,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1207,7 +1143,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1221,9 +1157,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B31">
         <v>45326</v>
@@ -1235,9 +1171,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B32">
         <v>45442</v>
@@ -1249,9 +1185,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B33">
         <v>45442</v>
@@ -1263,9 +1199,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B34">
         <v>45442</v>
@@ -1277,9 +1213,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B35">
         <v>45446</v>
@@ -1291,9 +1227,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B36">
         <v>45446</v>
@@ -1305,9 +1241,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B37">
         <v>45446</v>
@@ -1319,9 +1255,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B38">
         <v>45446</v>
@@ -1333,7 +1269,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -1347,7 +1283,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -1361,7 +1297,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -1375,7 +1311,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -1389,7 +1325,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -1403,7 +1339,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -1417,9 +1353,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B45">
         <v>45466</v>
@@ -1431,9 +1367,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B46">
         <v>45466</v>
@@ -1445,7 +1381,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -1459,9 +1395,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B48">
         <v>45466</v>
@@ -1473,9 +1409,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B49">
         <v>45471</v>
@@ -1487,9 +1423,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B50">
         <v>45471</v>
@@ -1501,9 +1437,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B51">
         <v>45472</v>
@@ -1515,7 +1451,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -1529,9 +1465,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B53">
         <v>45481</v>
@@ -1543,9 +1479,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B54">
         <v>45485</v>
@@ -1557,9 +1493,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B55">
         <v>45485</v>
@@ -1571,7 +1507,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -1585,7 +1521,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -1599,9 +1535,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B58">
         <v>45488</v>
@@ -1613,9 +1549,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B59">
         <v>45495</v>
@@ -1627,9 +1563,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B60">
         <v>45495</v>
@@ -1641,9 +1577,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B61">
         <v>45495</v>
@@ -1655,9 +1591,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B62">
         <v>45495</v>
@@ -1669,7 +1605,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -1683,7 +1619,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
         <v>5</v>
       </c>
@@ -1697,7 +1633,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>6</v>
       </c>
@@ -1711,9 +1647,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B66">
         <v>45497</v>
@@ -1725,7 +1661,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>7</v>
       </c>
@@ -1739,7 +1675,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>15</v>
       </c>
@@ -1753,9 +1689,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B69">
         <v>45518</v>
@@ -1767,9 +1703,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B70">
         <v>45518</v>
@@ -1781,9 +1717,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B71">
         <v>45518</v>
@@ -1795,9 +1731,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B72">
         <v>45518</v>
@@ -1809,7 +1745,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>14</v>
       </c>
@@ -1823,7 +1759,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>12</v>
       </c>
@@ -1837,7 +1773,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>13</v>
       </c>
@@ -1851,7 +1787,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>14</v>
       </c>
@@ -1865,7 +1801,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
         <v>15</v>
       </c>
@@ -1879,9 +1815,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B78">
         <v>45537</v>
@@ -1893,9 +1829,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B79">
         <v>45537</v>
@@ -1907,7 +1843,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
         <v>9</v>
       </c>
@@ -1921,9 +1857,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B81">
         <v>45587</v>
@@ -1935,9 +1871,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B82">
         <v>45587</v>
@@ -1949,9 +1885,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B83">
         <v>45594</v>
@@ -1963,9 +1899,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B84">
         <v>45594</v>
@@ -1977,9 +1913,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B85">
         <v>45599</v>
@@ -1991,9 +1927,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B86">
         <v>45599</v>
@@ -2005,9 +1941,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B87">
         <v>45609</v>
@@ -2019,7 +1955,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4">
       <c r="A88" t="s">
         <v>15</v>
       </c>
@@ -2033,7 +1969,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4">
       <c r="A89" t="s">
         <v>7</v>
       </c>
@@ -2047,7 +1983,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4">
       <c r="A90" t="s">
         <v>7</v>
       </c>
@@ -2061,7 +1997,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4">
       <c r="A91" t="s">
         <v>7</v>
       </c>
@@ -2075,7 +2011,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4">
       <c r="A92" t="s">
         <v>15</v>
       </c>
@@ -2089,7 +2025,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4">
       <c r="A93" t="s">
         <v>14</v>
       </c>
@@ -2103,9 +2039,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B94">
         <v>45617</v>
@@ -2117,7 +2053,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4">
       <c r="A95" t="s">
         <v>9</v>
       </c>
@@ -2131,7 +2067,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4">
       <c r="A96" t="s">
         <v>11</v>
       </c>
@@ -2145,9 +2081,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B97">
         <v>45617</v>
@@ -2159,7 +2095,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
         <v>11</v>
       </c>
@@ -2173,9 +2109,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B99">
         <v>45619</v>
@@ -2187,7 +2123,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4">
       <c r="A100" t="s">
         <v>9</v>
       </c>
@@ -2201,9 +2137,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B101">
         <v>45619</v>
@@ -2215,9 +2151,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B102">
         <v>45620</v>
@@ -2229,9 +2165,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B103">
         <v>45620</v>
@@ -2243,9 +2179,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B104">
         <v>45620</v>
@@ -2257,9 +2193,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B105">
         <v>45620</v>
@@ -2271,9 +2207,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B106">
         <v>45632</v>
@@ -2285,7 +2221,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4">
       <c r="A107" t="s">
         <v>7</v>
       </c>
@@ -2299,7 +2235,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4">
       <c r="A108" t="s">
         <v>10</v>
       </c>
@@ -2313,7 +2249,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4">
       <c r="A109" t="s">
         <v>9</v>
       </c>
@@ -2327,9 +2263,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B110">
         <v>45634</v>
@@ -2341,9 +2277,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B111">
         <v>45634</v>
@@ -2355,9 +2291,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4">
       <c r="A112" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B112">
         <v>45634</v>
@@ -2369,9 +2305,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B113">
         <v>45638</v>
@@ -2383,9 +2319,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B114">
         <v>45639</v>
@@ -2397,9 +2333,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B115">
         <v>45640</v>
@@ -2411,9 +2347,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B116">
         <v>45640</v>
@@ -2425,9 +2361,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B117">
         <v>45640</v>
@@ -2439,7 +2375,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4">
       <c r="A118" t="s">
         <v>14</v>
       </c>
@@ -2453,9 +2389,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B119">
         <v>45640</v>
@@ -2467,7 +2403,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4">
       <c r="A120" t="s">
         <v>15</v>
       </c>
@@ -2481,7 +2417,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4">
       <c r="A121" t="s">
         <v>7</v>
       </c>
@@ -2495,7 +2431,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4">
       <c r="A122" t="s">
         <v>14</v>
       </c>
@@ -2509,9 +2445,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B123">
         <v>45643</v>
@@ -2523,7 +2459,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4">
       <c r="A124" t="s">
         <v>15</v>
       </c>
@@ -2537,7 +2473,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4">
       <c r="A125" t="s">
         <v>7</v>
       </c>
@@ -2551,9 +2487,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B126">
         <v>45655</v>
@@ -2565,9 +2501,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4">
       <c r="A127" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B127">
         <v>45655</v>
@@ -2579,9 +2515,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4">
       <c r="A128" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B128">
         <v>45655</v>
@@ -2593,7 +2529,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4">
       <c r="A129" t="s">
         <v>14</v>
       </c>
@@ -2607,9 +2543,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4">
       <c r="A130" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B130">
         <v>45656</v>
@@ -2621,9 +2557,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4">
       <c r="A131" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B131">
         <v>45656</v>
@@ -2635,7 +2571,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4">
       <c r="A132" t="s">
         <v>7</v>
       </c>
@@ -2649,9 +2585,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4">
       <c r="A133" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B133">
         <v>45657</v>
@@ -2663,7 +2599,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4">
       <c r="A134" t="s">
         <v>9</v>
       </c>
@@ -2677,9 +2613,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4">
       <c r="A135" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B135">
         <v>45658</v>
@@ -2691,9 +2627,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4">
       <c r="A136" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B136">
         <v>45658</v>
@@ -2705,7 +2641,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4">
       <c r="A137" t="s">
         <v>14</v>
       </c>
@@ -2719,9 +2655,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4">
       <c r="A138" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B138">
         <v>45658</v>
@@ -2733,9 +2669,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4">
       <c r="A139" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B139">
         <v>45658</v>
@@ -2747,7 +2683,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4">
       <c r="A140" t="s">
         <v>13</v>
       </c>
@@ -2761,7 +2697,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4">
       <c r="A141" t="s">
         <v>12</v>
       </c>
@@ -2775,7 +2711,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4">
       <c r="A142" t="s">
         <v>9</v>
       </c>
@@ -2789,7 +2725,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4">
       <c r="A143" t="s">
         <v>8</v>
       </c>
@@ -2803,9 +2739,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4">
       <c r="A144" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B144">
         <v>45665</v>
@@ -2817,9 +2753,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4">
       <c r="A145" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B145">
         <v>45665</v>
@@ -2831,7 +2767,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4">
       <c r="A146" t="s">
         <v>14</v>
       </c>
@@ -2845,7 +2781,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4">
       <c r="A147" t="s">
         <v>15</v>
       </c>
@@ -2859,7 +2795,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4">
       <c r="A148" t="s">
         <v>14</v>
       </c>
@@ -2873,9 +2809,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4">
       <c r="A149" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B149">
         <v>45931</v>
@@ -2887,7 +2823,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4">
       <c r="A150" t="s">
         <v>15</v>
       </c>
@@ -2901,7 +2837,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4">
       <c r="A151" t="s">
         <v>14</v>
       </c>
@@ -2915,9 +2851,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4">
       <c r="A152" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B152">
         <v>45947</v>
@@ -2929,7 +2865,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4">
       <c r="A153" t="s">
         <v>6</v>
       </c>
@@ -2943,7 +2879,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4">
       <c r="A154" t="s">
         <v>5</v>
       </c>
@@ -2957,7 +2893,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4">
       <c r="A155" t="s">
         <v>7</v>
       </c>
@@ -2971,7 +2907,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4">
       <c r="A156" t="s">
         <v>5</v>
       </c>
@@ -2985,7 +2921,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4">
       <c r="A157" t="s">
         <v>6</v>
       </c>
@@ -2999,9 +2935,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4">
       <c r="A158" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B158">
         <v>46032</v>
@@ -3013,7 +2949,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4">
       <c r="A159" t="s">
         <v>15</v>
       </c>
@@ -3027,7 +2963,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4">
       <c r="A160" t="s">
         <v>7</v>
       </c>
@@ -3041,9 +2977,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4">
       <c r="A161" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B161">
         <v>46039</v>
@@ -3055,9 +2991,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4">
       <c r="A162" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B162">
         <v>46039</v>
@@ -3069,7 +3005,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4">
       <c r="A163" t="s">
         <v>11</v>
       </c>
@@ -3083,7 +3019,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4">
       <c r="A164" t="s">
         <v>8</v>
       </c>
@@ -3097,7 +3033,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4">
       <c r="A165" t="s">
         <v>9</v>
       </c>
@@ -3111,7 +3047,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4">
       <c r="A166" t="s">
         <v>10</v>
       </c>
@@ -3125,7 +3061,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4">
       <c r="A167" t="s">
         <v>7</v>
       </c>
@@ -3139,7 +3075,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4">
       <c r="A168" t="s">
         <v>15</v>
       </c>
@@ -3153,9 +3089,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4">
       <c r="A169" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B169">
         <v>46053</v>
@@ -3167,7 +3103,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4">
       <c r="A170" t="s">
         <v>14</v>
       </c>
@@ -3181,9 +3117,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4">
       <c r="A171" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B171">
         <v>46053</v>
@@ -3195,9 +3131,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4">
       <c r="A172" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B172">
         <v>46053</v>
@@ -3209,7 +3145,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4">
       <c r="A173" t="s">
         <v>15</v>
       </c>
@@ -3223,7 +3159,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4">
       <c r="A174" t="s">
         <v>15</v>
       </c>
@@ -3237,9 +3173,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4">
       <c r="A175" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B175">
         <v>46097</v>
@@ -3251,9 +3187,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4">
       <c r="A176" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B176">
         <v>46097</v>
@@ -3265,7 +3201,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5">
       <c r="A177" t="s">
         <v>7</v>
       </c>
@@ -3279,9 +3215,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5">
       <c r="A178" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B178">
         <v>40207</v>
@@ -3292,10 +3228,13 @@
       <c r="D178" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E178" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
       <c r="A179" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B179">
         <v>40207</v>
@@ -3306,8 +3245,11 @@
       <c r="D179" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E179" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
       <c r="A180" t="s">
         <v>14</v>
       </c>
@@ -3320,8 +3262,11 @@
       <c r="D180" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E180" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
       <c r="A181" t="s">
         <v>15</v>
       </c>
@@ -3334,8 +3279,11 @@
       <c r="D181" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E181" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
       <c r="A182" t="s">
         <v>7</v>
       </c>
@@ -3349,9 +3297,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5">
       <c r="A183" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B183">
         <v>42987</v>
@@ -3362,10 +3310,13 @@
       <c r="D183" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E183" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
       <c r="A184" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B184">
         <v>42987</v>
@@ -3376,8 +3327,11 @@
       <c r="D184" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E184" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
       <c r="A185" t="s">
         <v>7</v>
       </c>
@@ -3391,7 +3345,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5">
       <c r="A186" t="s">
         <v>15</v>
       </c>
@@ -3405,9 +3359,9 @@
         <v>116</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5">
       <c r="A187" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B187">
         <v>45825</v>

</xml_diff>

<commit_message>
disable tracking for non lootables
</commit_message>
<xml_diff>
--- a/data/players_priorities.xlsx
+++ b/data/players_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scripts\Divide-BiS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFF8836-05E6-4E19-9FCF-971D64C1C97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E544AB5A-DABA-4C15-A3ED-DCE675DCC0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="118">
   <si>
     <t>player</t>
   </si>
@@ -374,9 +374,6 @@
   </si>
   <si>
     <t>Emblems of Conquest</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
 </sst>
 </file>
@@ -780,7 +777,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E187"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="E163" sqref="E163"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1464,7 +1463,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -1478,7 +1477,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>13</v>
       </c>
@@ -1492,7 +1491,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -1506,7 +1505,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -1519,11 +1518,8 @@
       <c r="D52" t="s">
         <v>115</v>
       </c>
-      <c r="E52" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -1536,11 +1532,8 @@
       <c r="D53" t="s">
         <v>115</v>
       </c>
-      <c r="E53" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>11</v>
       </c>
@@ -1554,7 +1547,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>8</v>
       </c>
@@ -1568,7 +1561,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>15</v>
       </c>
@@ -1582,7 +1575,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>13</v>
       </c>
@@ -1596,7 +1589,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -1610,7 +1603,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -1624,7 +1617,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>7</v>
       </c>
@@ -1638,7 +1631,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>7</v>
       </c>
@@ -1652,7 +1645,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>7</v>
       </c>
@@ -1666,7 +1659,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>11</v>
       </c>
@@ -1680,7 +1673,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>12</v>
       </c>
@@ -1918,7 +1911,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>9</v>
       </c>
@@ -1932,7 +1925,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>15</v>
       </c>
@@ -1946,7 +1939,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>14</v>
       </c>
@@ -1960,7 +1953,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>13</v>
       </c>
@@ -1974,7 +1967,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>10</v>
       </c>
@@ -1988,7 +1981,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>12</v>
       </c>
@@ -2002,7 +1995,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>11</v>
       </c>
@@ -2016,7 +2009,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>11</v>
       </c>
@@ -2030,7 +2023,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>12</v>
       </c>
@@ -2044,7 +2037,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>11</v>
       </c>
@@ -2058,7 +2051,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>12</v>
       </c>
@@ -2072,7 +2065,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>9</v>
       </c>
@@ -2086,7 +2079,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>9</v>
       </c>
@@ -2099,11 +2092,8 @@
       <c r="D93" t="s">
         <v>115</v>
       </c>
-      <c r="E93" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>7</v>
       </c>
@@ -2116,11 +2106,8 @@
       <c r="D94" t="s">
         <v>115</v>
       </c>
-      <c r="E94" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>10</v>
       </c>
@@ -2134,7 +2121,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>7</v>
       </c>
@@ -3044,7 +3031,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>9</v>
       </c>
@@ -3058,7 +3045,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>6</v>
       </c>
@@ -3071,11 +3058,8 @@
       <c r="D162" t="s">
         <v>115</v>
       </c>
-      <c r="E162" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>5</v>
       </c>
@@ -3088,11 +3072,8 @@
       <c r="D163" t="s">
         <v>115</v>
       </c>
-      <c r="E163" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>11</v>
       </c>
@@ -3106,7 +3087,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>6</v>
       </c>
@@ -3120,7 +3101,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>6</v>
       </c>
@@ -3134,7 +3115,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>11</v>
       </c>
@@ -3148,7 +3129,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>7</v>
       </c>
@@ -3162,7 +3143,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>9</v>
       </c>
@@ -3176,7 +3157,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>9</v>
       </c>
@@ -3190,7 +3171,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>15</v>
       </c>
@@ -3204,7 +3185,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>13</v>
       </c>
@@ -3218,7 +3199,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>14</v>
       </c>
@@ -3232,7 +3213,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>10</v>
       </c>
@@ -3246,7 +3227,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>13</v>
       </c>
@@ -3260,7 +3241,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
add solo status to received column
</commit_message>
<xml_diff>
--- a/data/players_priorities.xlsx
+++ b/data/players_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scripts\Divide-BiS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080638EC-3CE8-4E67-8593-23039A7CAD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C7F325-5EFB-4C8D-A86A-BFBD41BABA4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="178">
   <si>
     <t>player</t>
   </si>
@@ -551,6 +551,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>SOLO</t>
   </si>
 </sst>
 </file>
@@ -955,7 +958,7 @@
   <dimension ref="A1:E421"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="E104" sqref="E104"/>
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2465,6 +2468,9 @@
       <c r="D105" t="s">
         <v>164</v>
       </c>
+      <c r="E105" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">

</xml_diff>

<commit_message>
convert crafts to lootable
</commit_message>
<xml_diff>
--- a/data/players_priorities.xlsx
+++ b/data/players_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scripts\Divide-BiS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DF6E82-0DC0-4CE5-825B-5D75F94286D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF7F087-49DE-48EF-838F-D8B3FB2DB362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="178">
   <si>
     <t>player</t>
   </si>
@@ -957,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E421"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="E162" sqref="E162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1153,6 +1153,9 @@
       <c r="D13" t="s">
         <v>160</v>
       </c>
+      <c r="E13" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -3263,6 +3266,9 @@
       </c>
       <c r="D161" t="s">
         <v>160</v>
+      </c>
+      <c r="E161" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
switch emblems tokens to solo
</commit_message>
<xml_diff>
--- a/data/players_priorities.xlsx
+++ b/data/players_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scripts\Divide-BiS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3161BDB9-0698-451D-96AD-677497A78815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B388762-2B2E-4A60-897C-AF2B63FEF2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -963,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E387"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1550,7 +1550,7 @@
         <v>157</v>
       </c>
       <c r="E40" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1649,7 +1649,7 @@
         <v>159</v>
       </c>
       <c r="E46" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -2207,7 +2207,7 @@
         <v>157</v>
       </c>
       <c r="E85" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -2224,7 +2224,7 @@
         <v>158</v>
       </c>
       <c r="E86" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -2289,7 +2289,7 @@
         <v>158</v>
       </c>
       <c r="E90" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
@@ -2323,7 +2323,7 @@
         <v>157</v>
       </c>
       <c r="E92" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
@@ -2374,7 +2374,7 @@
         <v>160</v>
       </c>
       <c r="E95" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
change item_id query to exact match
</commit_message>
<xml_diff>
--- a/data/players_priorities.xlsx
+++ b/data/players_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scripts\Divide-BiS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A75322E-15A5-4ACA-8013-2F01317473D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0BE631-3FC8-429A-A57D-97031779067C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="187">
   <si>
     <t>player</t>
   </si>
@@ -951,7 +951,7 @@
   <dimension ref="A1:E372"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A272" workbookViewId="0">
-      <selection activeCell="O281" sqref="O281"/>
+      <selection activeCell="E287" sqref="E287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5040,6 +5040,9 @@
       <c r="D286" t="s">
         <v>143</v>
       </c>
+      <c r="E286" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A287" t="s">

</xml_diff>

<commit_message>
up 10/07 missing loots
</commit_message>
<xml_diff>
--- a/data/players_priorities.xlsx
+++ b/data/players_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scripts\Divide-BiS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEBF970-F817-4930-B0DE-96903D383768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7403C1E-5E57-4CF3-B3A7-74F5F10BCB41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="189">
   <si>
     <t>player</t>
   </si>
@@ -956,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E389"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
-      <selection activeCell="E232" sqref="E232"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1362,6 +1362,9 @@
       <c r="D28" t="s">
         <v>146</v>
       </c>
+      <c r="E28" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -1987,6 +1990,9 @@
       </c>
       <c r="D71" t="s">
         <v>145</v>
+      </c>
+      <c r="E71" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
up missing loot 12/07
</commit_message>
<xml_diff>
--- a/data/players_priorities.xlsx
+++ b/data/players_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scripts\Divide-BiS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD1780C-DB69-4E23-A243-DE814FDA1A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C924FD12-D843-4F64-BDFC-EB15EC9E2CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="187">
   <si>
     <t>player</t>
   </si>
@@ -950,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E372"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
-      <selection activeCell="E247" sqref="E247"/>
+    <sheetView tabSelected="1" topLeftCell="A310" workbookViewId="0">
+      <selection activeCell="E323" sqref="E323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5697,6 +5697,9 @@
       <c r="D322" t="s">
         <v>143</v>
       </c>
+      <c r="E322" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A323" t="s">

</xml_diff>

<commit_message>
add missing loots again 12/07
</commit_message>
<xml_diff>
--- a/data/players_priorities.xlsx
+++ b/data/players_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scripts\Divide-BiS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C924FD12-D843-4F64-BDFC-EB15EC9E2CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F6AB13-4E6D-459A-BA8B-39D3EAA252BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="187">
   <si>
     <t>player</t>
   </si>
@@ -950,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E372"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A310" workbookViewId="0">
-      <selection activeCell="E323" sqref="E323"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="I128" sqref="I128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2025,6 +2025,9 @@
       <c r="D73" t="s">
         <v>143</v>
       </c>
+      <c r="E73" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
@@ -2803,6 +2806,9 @@
       </c>
       <c r="D125" t="s">
         <v>143</v>
+      </c>
+      <c r="E125" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fix token loot attrib
</commit_message>
<xml_diff>
--- a/data/players_priorities.xlsx
+++ b/data/players_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dev\Divide-BiS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63AE00A-4698-4BAE-AAF7-0CCD58822F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8091ADD6-A4E6-4769-8948-99BD890CB737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="17400" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1001,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
-      <selection activeCell="F305" sqref="F305"/>
+    <sheetView tabSelected="1" topLeftCell="A289" workbookViewId="0">
+      <selection activeCell="F315" sqref="F315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5714,9 +5714,6 @@
       <c r="D304" t="s">
         <v>190</v>
       </c>
-      <c r="E304" t="s">
-        <v>203</v>
-      </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
@@ -5820,6 +5817,9 @@
       </c>
       <c r="D311" t="s">
         <v>197</v>
+      </c>
+      <c r="E311" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add skotia, fuldrak, nordton
</commit_message>
<xml_diff>
--- a/data/players_priorities.xlsx
+++ b/data/players_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Divide-BiS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA07B85B-C08E-4030-A040-A31AC4B83BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E06A71-CD82-4488-9DA7-96F813ED7EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="91">
   <si>
     <t>player</t>
   </si>
@@ -37,21 +37,30 @@
     <t>received</t>
   </si>
   <si>
+    <t>Fuldrak</t>
+  </si>
+  <si>
+    <t>Aldriana's Gloves of Secrecy</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Nordton</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>Mokà</t>
   </si>
   <si>
     <t>Althor's Abacus</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Linacool</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Skotia</t>
   </si>
   <si>
@@ -67,6 +76,9 @@
     <t>Reputation</t>
   </si>
   <si>
+    <t>Ashen Band of Endless Vengeance</t>
+  </si>
+  <si>
     <t>Ashen Band of Endless Wisdom</t>
   </si>
   <si>
@@ -136,6 +148,9 @@
     <t>Deathbringer's Will</t>
   </si>
   <si>
+    <t>Fal'inrush, Defender of Quel'thalas</t>
+  </si>
+  <si>
     <t>Fallen Lord's Handguards</t>
   </si>
   <si>
@@ -145,9 +160,15 @@
     <t>Frostbinder's Shredded Cape</t>
   </si>
   <si>
+    <t>Frostbrood Sapphire Ring</t>
+  </si>
+  <si>
     <t>Gendarme's Cuirass</t>
   </si>
   <si>
+    <t>Glorenzelg, High-Blade of the Silver Hand</t>
+  </si>
+  <si>
     <t>Greatcloak of the Turned Champion</t>
   </si>
   <si>
@@ -178,6 +199,9 @@
     <t>Lingering Illness</t>
   </si>
   <si>
+    <t>Marrowgar's Frigid Eye</t>
+  </si>
+  <si>
     <t>Memory of Malygos</t>
   </si>
   <si>
@@ -193,6 +217,15 @@
     <t>Professor's Bloodied Smock</t>
   </si>
   <si>
+    <t>Protector's Mark of Sanctification</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
     <t>Raging Behemoth's Shoulderplates</t>
   </si>
   <si>
@@ -211,12 +244,21 @@
     <t>Scourge Reaver's Legplates</t>
   </si>
   <si>
+    <t>Shadowmourne</t>
+  </si>
+  <si>
+    <t>Legendary</t>
+  </si>
+  <si>
     <t>Sigil of Virulence</t>
   </si>
   <si>
     <t>Emblems of Triumph</t>
   </si>
   <si>
+    <t>Sindragosa's Cruel Claw</t>
+  </si>
+  <si>
     <t>Skeleton Lord's Circle</t>
   </si>
   <si>
@@ -232,19 +274,22 @@
     <t>Taiga Bindings</t>
   </si>
   <si>
+    <t>Toskk's Maximized Wristguards</t>
+  </si>
+  <si>
     <t>Val'anyr, Hammer of Ancient Kings</t>
   </si>
   <si>
-    <t>Legendary</t>
-  </si>
-  <si>
     <t>Vanquisher's Mark of Sanctification</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
+    <t>Vereesa's Dexterity</t>
+  </si>
+  <si>
+    <t>Warmace of Menethil</t>
+  </si>
+  <si>
+    <t>Whispering Fanged Skull</t>
   </si>
   <si>
     <t>Winding Sheet</t>
@@ -610,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:E120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,7 +685,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>50366</v>
+        <v>50675</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -654,7 +699,7 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>50366</v>
+        <v>50675</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -671,10 +716,10 @@
         <v>50366</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -682,24 +727,24 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>52572</v>
+        <v>50366</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B6">
-        <v>50400</v>
+        <v>50366</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -707,125 +752,125 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B7">
-        <v>50400</v>
+        <v>52572</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>50400</v>
+        <v>50402</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>50400</v>
+        <v>50402</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B10">
-        <v>49894</v>
+        <v>50400</v>
       </c>
       <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
         <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>50724</v>
+        <v>50400</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B12">
-        <v>50639</v>
+        <v>50400</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>50609</v>
+        <v>49894</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B14">
-        <v>50609</v>
+        <v>50724</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>50630</v>
+        <v>50639</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -833,13 +878,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B16">
-        <v>50630</v>
+        <v>50639</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
@@ -847,47 +892,44 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B17">
-        <v>50616</v>
+        <v>50639</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B18">
-        <v>47146</v>
+        <v>50609</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
-      </c>
-      <c r="E18" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B19">
-        <v>50620</v>
+        <v>50609</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -895,10 +937,10 @@
         <v>12</v>
       </c>
       <c r="B20">
-        <v>51842</v>
+        <v>50630</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
@@ -906,97 +948,100 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B21">
-        <v>52030</v>
+        <v>50630</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>52030</v>
+        <v>50616</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B23">
-        <v>52030</v>
+        <v>47146</v>
       </c>
       <c r="C23" t="s">
         <v>28</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B24">
-        <v>52030</v>
+        <v>50620</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D24" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B25">
-        <v>52030</v>
+        <v>50620</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B26">
-        <v>52030</v>
+        <v>50620</v>
       </c>
       <c r="C26" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27">
-        <v>51928</v>
+        <v>51842</v>
       </c>
       <c r="C27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
@@ -1004,13 +1049,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B28">
-        <v>50613</v>
+        <v>52030</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
@@ -1018,512 +1063,509 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B29">
-        <v>50721</v>
+        <v>52030</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B30">
-        <v>50686</v>
+        <v>52030</v>
       </c>
       <c r="C30" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B31">
-        <v>47131</v>
+        <v>52030</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B32">
+        <v>52030</v>
+      </c>
+      <c r="C32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33">
+        <v>52030</v>
+      </c>
+      <c r="C33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <v>51928</v>
+      </c>
+      <c r="C34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35">
+        <v>50613</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36">
+        <v>50721</v>
+      </c>
+      <c r="C36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37">
+        <v>50686</v>
+      </c>
+      <c r="C37" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38">
+        <v>47131</v>
+      </c>
+      <c r="C38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39">
         <v>50363</v>
       </c>
-      <c r="C32" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33">
-        <v>50650</v>
-      </c>
-      <c r="C33" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34">
-        <v>50690</v>
-      </c>
-      <c r="C34" t="s">
-        <v>39</v>
-      </c>
-      <c r="D34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="C39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>5</v>
       </c>
-      <c r="B35">
-        <v>50628</v>
-      </c>
-      <c r="C35" t="s">
-        <v>40</v>
-      </c>
-      <c r="D35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>16</v>
-      </c>
-      <c r="B36">
-        <v>50628</v>
-      </c>
-      <c r="C36" t="s">
-        <v>40</v>
-      </c>
-      <c r="D36" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37">
-        <v>50606</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="B40">
+        <v>50363</v>
+      </c>
+      <c r="C40" t="s">
         <v>41</v>
       </c>
-      <c r="D37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>8</v>
       </c>
-      <c r="B38">
-        <v>50668</v>
-      </c>
-      <c r="C38" t="s">
-        <v>42</v>
-      </c>
-      <c r="D38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>10</v>
-      </c>
-      <c r="B39">
-        <v>50668</v>
-      </c>
-      <c r="C39" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40">
-        <v>50737</v>
-      </c>
-      <c r="C40" t="s">
-        <v>43</v>
-      </c>
-      <c r="D40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>12</v>
-      </c>
       <c r="B41">
-        <v>50737</v>
+        <v>50363</v>
       </c>
       <c r="C41" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D41" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>5</v>
       </c>
       <c r="B42">
-        <v>50700</v>
+        <v>50733</v>
       </c>
       <c r="C42" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D42" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>8</v>
       </c>
       <c r="B43">
-        <v>50454</v>
+        <v>50733</v>
       </c>
       <c r="C43" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44">
+        <v>50650</v>
+      </c>
+      <c r="C44" t="s">
+        <v>43</v>
+      </c>
+      <c r="D44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45">
+        <v>50690</v>
+      </c>
+      <c r="C45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46">
+        <v>50628</v>
+      </c>
+      <c r="C46" t="s">
         <v>45</v>
       </c>
-      <c r="D43" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>10</v>
-      </c>
-      <c r="B44">
-        <v>50454</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="D46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47">
+        <v>50628</v>
+      </c>
+      <c r="C47" t="s">
         <v>45</v>
       </c>
-      <c r="D44" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>5</v>
-      </c>
-      <c r="B45">
-        <v>51882</v>
-      </c>
-      <c r="C45" t="s">
-        <v>47</v>
-      </c>
-      <c r="D45" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>12</v>
-      </c>
-      <c r="B46">
-        <v>50712</v>
-      </c>
-      <c r="C46" t="s">
-        <v>48</v>
-      </c>
-      <c r="D46" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>16</v>
-      </c>
-      <c r="B47">
-        <v>40705</v>
-      </c>
-      <c r="C47" t="s">
-        <v>49</v>
-      </c>
       <c r="D47" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>5</v>
       </c>
       <c r="B48">
-        <v>50702</v>
+        <v>50618</v>
       </c>
       <c r="C48" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D48" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>8</v>
       </c>
       <c r="B49">
-        <v>50636</v>
+        <v>50618</v>
       </c>
       <c r="C49" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D49" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B50">
-        <v>50636</v>
+        <v>50606</v>
       </c>
       <c r="C50" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D50" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B51">
-        <v>46051</v>
+        <v>50730</v>
       </c>
       <c r="C51" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D51" t="s">
         <v>7</v>
       </c>
-      <c r="E51" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B52">
-        <v>50631</v>
+        <v>50730</v>
       </c>
       <c r="C52" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D52" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B53">
-        <v>50699</v>
+        <v>50668</v>
       </c>
       <c r="C53" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D53" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B54">
-        <v>50699</v>
+        <v>50668</v>
       </c>
       <c r="C54" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D54" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B55">
-        <v>50699</v>
+        <v>50737</v>
       </c>
       <c r="C55" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D55" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B56">
-        <v>50705</v>
+        <v>50737</v>
       </c>
       <c r="C56" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D56" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>10</v>
       </c>
       <c r="B57">
-        <v>50705</v>
+        <v>50700</v>
       </c>
       <c r="C57" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D57" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>12</v>
       </c>
       <c r="B58">
-        <v>50674</v>
+        <v>50454</v>
       </c>
       <c r="C58" t="s">
+        <v>52</v>
+      </c>
+      <c r="D58" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59">
+        <v>50454</v>
+      </c>
+      <c r="C59" t="s">
+        <v>52</v>
+      </c>
+      <c r="D59" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60">
+        <v>51882</v>
+      </c>
+      <c r="C60" t="s">
+        <v>54</v>
+      </c>
+      <c r="D60" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>15</v>
+      </c>
+      <c r="B61">
+        <v>50712</v>
+      </c>
+      <c r="C61" t="s">
+        <v>55</v>
+      </c>
+      <c r="D61" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62">
+        <v>40705</v>
+      </c>
+      <c r="C62" t="s">
+        <v>56</v>
+      </c>
+      <c r="D62" t="s">
         <v>57</v>
       </c>
-      <c r="D58" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>5</v>
-      </c>
-      <c r="B59">
-        <v>50664</v>
-      </c>
-      <c r="C59" t="s">
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63">
+        <v>50702</v>
+      </c>
+      <c r="C63" t="s">
         <v>58</v>
       </c>
-      <c r="D59" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>16</v>
-      </c>
-      <c r="B60">
-        <v>50664</v>
-      </c>
-      <c r="C60" t="s">
-        <v>58</v>
-      </c>
-      <c r="D60" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>16</v>
-      </c>
-      <c r="B61">
-        <v>50680</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="D63" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>13</v>
+      </c>
+      <c r="B64">
+        <v>50610</v>
+      </c>
+      <c r="C64" t="s">
         <v>59</v>
       </c>
-      <c r="D61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>5</v>
-      </c>
-      <c r="B62">
-        <v>50734</v>
-      </c>
-      <c r="C62" t="s">
-        <v>60</v>
-      </c>
-      <c r="D62" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>8</v>
-      </c>
-      <c r="B63">
-        <v>50717</v>
-      </c>
-      <c r="C63" t="s">
-        <v>61</v>
-      </c>
-      <c r="D63" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>10</v>
-      </c>
-      <c r="B64">
-        <v>50717</v>
-      </c>
-      <c r="C64" t="s">
-        <v>61</v>
-      </c>
       <c r="D64" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -1531,10 +1573,10 @@
         <v>12</v>
       </c>
       <c r="B65">
-        <v>50624</v>
+        <v>50636</v>
       </c>
       <c r="C65" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D65" t="s">
         <v>7</v>
@@ -1542,41 +1584,44 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B66">
-        <v>47673</v>
+        <v>50636</v>
       </c>
       <c r="C66" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D66" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B67">
-        <v>50657</v>
+        <v>46051</v>
       </c>
       <c r="C67" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D67" t="s">
         <v>7</v>
+      </c>
+      <c r="E67" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B68">
-        <v>47059</v>
+        <v>50631</v>
       </c>
       <c r="C68" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D68" t="s">
         <v>7</v>
@@ -1584,61 +1629,55 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B69">
-        <v>47059</v>
+        <v>50699</v>
       </c>
       <c r="C69" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D69" t="s">
-        <v>9</v>
-      </c>
-      <c r="E69" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B70">
-        <v>47059</v>
+        <v>50699</v>
       </c>
       <c r="C70" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D70" t="s">
-        <v>11</v>
-      </c>
-      <c r="E70" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B71">
-        <v>37111</v>
+        <v>50699</v>
       </c>
       <c r="C71" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D71" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B72">
-        <v>50635</v>
+        <v>50705</v>
       </c>
       <c r="C72" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D72" t="s">
         <v>7</v>
@@ -1646,13 +1685,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B73">
-        <v>50635</v>
+        <v>50705</v>
       </c>
       <c r="C73" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D73" t="s">
         <v>9</v>
@@ -1660,13 +1699,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B74">
-        <v>51832</v>
+        <v>52029</v>
       </c>
       <c r="C74" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D74" t="s">
         <v>7</v>
@@ -1674,53 +1713,44 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B75">
-        <v>46017</v>
+        <v>52029</v>
       </c>
       <c r="C75" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D75" t="s">
-        <v>71</v>
-      </c>
-      <c r="E75" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B76">
-        <v>46017</v>
+        <v>52029</v>
       </c>
       <c r="C76" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D76" t="s">
-        <v>71</v>
-      </c>
-      <c r="E76" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B77">
-        <v>46017</v>
+        <v>52029</v>
       </c>
       <c r="C77" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D77" t="s">
-        <v>71</v>
-      </c>
-      <c r="E77" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
@@ -1728,13 +1758,13 @@
         <v>8</v>
       </c>
       <c r="B78">
-        <v>52028</v>
+        <v>52029</v>
       </c>
       <c r="C78" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D78" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -1742,13 +1772,13 @@
         <v>8</v>
       </c>
       <c r="B79">
-        <v>52028</v>
+        <v>52029</v>
       </c>
       <c r="C79" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D79" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -1756,96 +1786,587 @@
         <v>8</v>
       </c>
       <c r="B80">
-        <v>52028</v>
+        <v>52029</v>
       </c>
       <c r="C80" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D80" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>8</v>
       </c>
       <c r="B81">
-        <v>52028</v>
+        <v>52029</v>
       </c>
       <c r="C81" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D81" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B82">
-        <v>52028</v>
+        <v>50674</v>
       </c>
       <c r="C82" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D82" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>10</v>
       </c>
       <c r="B83">
+        <v>50664</v>
+      </c>
+      <c r="C83" t="s">
+        <v>69</v>
+      </c>
+      <c r="D83" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>20</v>
+      </c>
+      <c r="B84">
+        <v>50664</v>
+      </c>
+      <c r="C84" t="s">
+        <v>69</v>
+      </c>
+      <c r="D84" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>20</v>
+      </c>
+      <c r="B85">
+        <v>50680</v>
+      </c>
+      <c r="C85" t="s">
+        <v>70</v>
+      </c>
+      <c r="D85" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>10</v>
+      </c>
+      <c r="B86">
+        <v>50734</v>
+      </c>
+      <c r="C86" t="s">
+        <v>71</v>
+      </c>
+      <c r="D86" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>12</v>
+      </c>
+      <c r="B87">
+        <v>50717</v>
+      </c>
+      <c r="C87" t="s">
+        <v>72</v>
+      </c>
+      <c r="D87" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>13</v>
+      </c>
+      <c r="B88">
+        <v>50717</v>
+      </c>
+      <c r="C88" t="s">
+        <v>72</v>
+      </c>
+      <c r="D88" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>15</v>
+      </c>
+      <c r="B89">
+        <v>50624</v>
+      </c>
+      <c r="C89" t="s">
+        <v>73</v>
+      </c>
+      <c r="D89" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>8</v>
+      </c>
+      <c r="B90">
+        <v>49623</v>
+      </c>
+      <c r="C90" t="s">
+        <v>74</v>
+      </c>
+      <c r="D90" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>15</v>
+      </c>
+      <c r="B91">
+        <v>47673</v>
+      </c>
+      <c r="C91" t="s">
+        <v>76</v>
+      </c>
+      <c r="D91" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>5</v>
+      </c>
+      <c r="B92">
+        <v>50633</v>
+      </c>
+      <c r="C92" t="s">
+        <v>78</v>
+      </c>
+      <c r="D92" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>8</v>
+      </c>
+      <c r="B93">
+        <v>50633</v>
+      </c>
+      <c r="C93" t="s">
+        <v>78</v>
+      </c>
+      <c r="D93" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>15</v>
+      </c>
+      <c r="B94">
+        <v>50657</v>
+      </c>
+      <c r="C94" t="s">
+        <v>79</v>
+      </c>
+      <c r="D94" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>12</v>
+      </c>
+      <c r="B95">
+        <v>47059</v>
+      </c>
+      <c r="C95" t="s">
+        <v>80</v>
+      </c>
+      <c r="D95" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>10</v>
+      </c>
+      <c r="B96">
+        <v>47059</v>
+      </c>
+      <c r="C96" t="s">
+        <v>80</v>
+      </c>
+      <c r="D96" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>13</v>
+      </c>
+      <c r="B97">
+        <v>47059</v>
+      </c>
+      <c r="C97" t="s">
+        <v>80</v>
+      </c>
+      <c r="D97" t="s">
+        <v>14</v>
+      </c>
+      <c r="E97" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>20</v>
+      </c>
+      <c r="B98">
+        <v>37111</v>
+      </c>
+      <c r="C98" t="s">
+        <v>81</v>
+      </c>
+      <c r="D98" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>12</v>
+      </c>
+      <c r="B99">
+        <v>50635</v>
+      </c>
+      <c r="C99" t="s">
+        <v>82</v>
+      </c>
+      <c r="D99" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>13</v>
+      </c>
+      <c r="B100">
+        <v>50635</v>
+      </c>
+      <c r="C100" t="s">
+        <v>82</v>
+      </c>
+      <c r="D100" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>15</v>
+      </c>
+      <c r="B101">
+        <v>51832</v>
+      </c>
+      <c r="C101" t="s">
+        <v>83</v>
+      </c>
+      <c r="D101" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>5</v>
+      </c>
+      <c r="B102">
+        <v>50670</v>
+      </c>
+      <c r="C102" t="s">
+        <v>84</v>
+      </c>
+      <c r="D102" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>8</v>
+      </c>
+      <c r="B103">
+        <v>50670</v>
+      </c>
+      <c r="C103" t="s">
+        <v>84</v>
+      </c>
+      <c r="D103" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>12</v>
+      </c>
+      <c r="B104">
+        <v>46017</v>
+      </c>
+      <c r="C104" t="s">
+        <v>85</v>
+      </c>
+      <c r="D104" t="s">
+        <v>75</v>
+      </c>
+      <c r="E104" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>20</v>
+      </c>
+      <c r="B105">
+        <v>46017</v>
+      </c>
+      <c r="C105" t="s">
+        <v>85</v>
+      </c>
+      <c r="D105" t="s">
+        <v>75</v>
+      </c>
+      <c r="E105" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>13</v>
+      </c>
+      <c r="B106">
+        <v>46017</v>
+      </c>
+      <c r="C106" t="s">
+        <v>85</v>
+      </c>
+      <c r="D106" t="s">
+        <v>75</v>
+      </c>
+      <c r="E106" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>12</v>
+      </c>
+      <c r="B107">
         <v>52028</v>
       </c>
-      <c r="C83" t="s">
-        <v>72</v>
-      </c>
-      <c r="D83" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>10</v>
-      </c>
-      <c r="B84">
+      <c r="C107" t="s">
+        <v>86</v>
+      </c>
+      <c r="D107" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>12</v>
+      </c>
+      <c r="B108">
         <v>52028</v>
       </c>
-      <c r="C84" t="s">
-        <v>72</v>
-      </c>
-      <c r="D84" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>10</v>
-      </c>
-      <c r="B85">
+      <c r="C108" t="s">
+        <v>86</v>
+      </c>
+      <c r="D108" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>12</v>
+      </c>
+      <c r="B109">
         <v>52028</v>
       </c>
-      <c r="C85" t="s">
-        <v>72</v>
-      </c>
-      <c r="D85" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+      <c r="C109" t="s">
+        <v>86</v>
+      </c>
+      <c r="D109" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
         <v>12</v>
       </c>
-      <c r="B86">
+      <c r="B110">
+        <v>52028</v>
+      </c>
+      <c r="C110" t="s">
+        <v>86</v>
+      </c>
+      <c r="D110" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>13</v>
+      </c>
+      <c r="B111">
+        <v>52028</v>
+      </c>
+      <c r="C111" t="s">
+        <v>86</v>
+      </c>
+      <c r="D111" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>13</v>
+      </c>
+      <c r="B112">
+        <v>52028</v>
+      </c>
+      <c r="C112" t="s">
+        <v>86</v>
+      </c>
+      <c r="D112" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>13</v>
+      </c>
+      <c r="B113">
+        <v>52028</v>
+      </c>
+      <c r="C113" t="s">
+        <v>86</v>
+      </c>
+      <c r="D113" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>13</v>
+      </c>
+      <c r="B114">
+        <v>52028</v>
+      </c>
+      <c r="C114" t="s">
+        <v>86</v>
+      </c>
+      <c r="D114" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>5</v>
+      </c>
+      <c r="B115">
+        <v>47545</v>
+      </c>
+      <c r="C115" t="s">
+        <v>87</v>
+      </c>
+      <c r="D115" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>8</v>
+      </c>
+      <c r="B116">
+        <v>47545</v>
+      </c>
+      <c r="C116" t="s">
+        <v>87</v>
+      </c>
+      <c r="D116" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>5</v>
+      </c>
+      <c r="B117">
+        <v>51946</v>
+      </c>
+      <c r="C117" t="s">
+        <v>88</v>
+      </c>
+      <c r="D117" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>5</v>
+      </c>
+      <c r="B118">
+        <v>50343</v>
+      </c>
+      <c r="C118" t="s">
+        <v>89</v>
+      </c>
+      <c r="D118" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>8</v>
+      </c>
+      <c r="B119">
+        <v>50343</v>
+      </c>
+      <c r="C119" t="s">
+        <v>89</v>
+      </c>
+      <c r="D119" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>15</v>
+      </c>
+      <c r="B120">
         <v>50677</v>
       </c>
-      <c r="C86" t="s">
-        <v>75</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="C120" t="s">
+        <v>90</v>
+      </c>
+      <c r="D120" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>